<commit_message>
digestion y ligacion mLSS y mSC5D
</commit_message>
<xml_diff>
--- a/Plantillas/Inventario almacen.xlsx
+++ b/Plantillas/Inventario almacen.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lemon\Desktop\IMDEA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marta.torrecilla\Desktop\IMDEA-2\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEB2184-C42D-4A00-A139-8F392480FF51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -152,9 +153,6 @@
     <t>LPDS (FBS delipidated)</t>
   </si>
   <si>
-    <t>Buffer de Laemmli (sample buffer / buffer carga)</t>
-  </si>
-  <si>
     <t>Glycine (Scharlab)</t>
   </si>
   <si>
@@ -300,12 +298,15 @@
   </si>
   <si>
     <t>T4 DNA ligasa (Thermo Fisher)</t>
+  </si>
+  <si>
+    <t>Dynabeads</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -603,38 +604,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="justify"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="255" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="255" shrinkToFit="1"/>
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="255" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="255" shrinkToFit="1"/>
     </xf>
@@ -656,13 +650,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="255" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="255" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="255" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -943,54 +944,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45:G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="5.21875" customWidth="1"/>
-    <col min="5" max="5" width="55.21875" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="53.28515625" customWidth="1"/>
+    <col min="2" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" customWidth="1"/>
+    <col min="5" max="5" width="55.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:7" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:7" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="29"/>
+      <c r="E2" s="27"/>
       <c r="F2" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
-      <c r="D3" s="37" t="s">
-        <v>76</v>
+      <c r="D3" s="36" t="s">
+        <v>75</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>4</v>
@@ -998,602 +998,597 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="21" t="s">
+      <c r="D4" s="37"/>
+      <c r="E4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="37"/>
+      <c r="E5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D6" s="37"/>
+      <c r="E6" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
-      <c r="D7" s="38"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
-      <c r="D8" s="38"/>
+      <c r="D8" s="37"/>
       <c r="E8" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="37"/>
+      <c r="E9" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="38"/>
-      <c r="E10" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
-      <c r="D12" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="29"/>
+      <c r="E12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="2" t="s">
-        <v>41</v>
+      <c r="D13" s="29"/>
+      <c r="E13" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="29"/>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="29"/>
+      <c r="E15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="2" t="s">
-        <v>11</v>
+      <c r="D16" s="29"/>
+      <c r="E16" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
-      <c r="D17" s="30"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="29"/>
+      <c r="E18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="2" t="s">
-        <v>15</v>
+      <c r="D19" s="29"/>
+      <c r="E19" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="29"/>
+      <c r="E20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="30"/>
-      <c r="E21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
-      <c r="D23" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="32"/>
+      <c r="E23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="32"/>
+      <c r="E24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D26" s="34"/>
+      <c r="E26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="35"/>
+      <c r="D27" s="34"/>
       <c r="E27" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
       <c r="D28" s="35"/>
-      <c r="E28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:7" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D31" s="37"/>
+      <c r="E31" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-    </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="37"/>
+      <c r="E32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="38"/>
+      <c r="D33" s="37"/>
       <c r="E33" s="1" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="23" t="s">
-        <v>75</v>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>74</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="1" t="s">
-        <v>89</v>
+      <c r="D34" s="37"/>
+      <c r="E34" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="38"/>
+      <c r="D35" s="37"/>
       <c r="E35" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="10" t="s">
-        <v>14</v>
+      <c r="D36" s="37"/>
+      <c r="E36" s="23" t="s">
+        <v>13</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="24" t="s">
-        <v>13</v>
+      <c r="D37" s="37"/>
+      <c r="E37" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="38"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="1" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="38"/>
+      <c r="D39" s="37"/>
       <c r="E39" s="1" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="38"/>
+      <c r="D40" s="37"/>
       <c r="E40" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="38"/>
+      <c r="D41" s="37"/>
       <c r="E41" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D42" s="37"/>
+      <c r="E42" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D43" s="37"/>
+      <c r="E43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="38"/>
+      <c r="D44" s="40"/>
       <c r="E44" s="1" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19"/>
       <c r="B45" s="19"/>
       <c r="C45" s="19"/>
-      <c r="D45" s="43"/>
+      <c r="D45" s="41" t="s">
+        <v>80</v>
+      </c>
       <c r="E45" s="1" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
       <c r="B46" s="19"/>
       <c r="C46" s="19"/>
-      <c r="D46" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>35</v>
+      <c r="D46" s="42"/>
+      <c r="E46" s="20" t="s">
+        <v>44</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D47" s="26"/>
-      <c r="E47" s="20" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D47" s="42"/>
+      <c r="E47" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D48" s="26"/>
-      <c r="E48" s="1" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D48" s="42"/>
+      <c r="E48" s="25" t="s">
         <v>46</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D49" s="26"/>
-      <c r="E49" s="41" t="s">
-        <v>47</v>
+    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D49" s="42"/>
+      <c r="E49" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D50" s="27"/>
+    <row r="50" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D50" s="43"/>
       <c r="E50" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="52" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E52" s="19"/>
-    </row>
-    <row r="53" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E53" s="19"/>
-    </row>
+    <row r="51" spans="4:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="D30:D44"/>
+    <mergeCell ref="D45:D50"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D12:D22"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="D3:D11"/>
-    <mergeCell ref="D31:D45"/>
-    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="D11:D21"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="D3:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>